<commit_message>
revisi field dosen tetap bagian admin
</commit_message>
<xml_diff>
--- a/public/contoh-excel/dosentetap.xlsx
+++ b/public/contoh-excel/dosentetap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>email</t>
   </si>
@@ -64,13 +64,31 @@
     <t>nominal_honor_mengajar_kls_malam</t>
   </si>
   <si>
-    <t>pmb_atau_penguji_kp</t>
-  </si>
-  <si>
-    <t>x_pmb_atau_penguji_kp</t>
-  </si>
-  <si>
-    <t>nominal_pmb_atau_penguji_kp</t>
+    <t>koordinator_matkul</t>
+  </si>
+  <si>
+    <t>x_koordinator_matkul</t>
+  </si>
+  <si>
+    <t>nominal_koordinator_matkul</t>
+  </si>
+  <si>
+    <t>koor_anggota_mbkm</t>
+  </si>
+  <si>
+    <t>x_koor_anggota_mbkm</t>
+  </si>
+  <si>
+    <t>nominal_koor_anggota_mbkm</t>
+  </si>
+  <si>
+    <t>pmb_atau_penguji_mbkm</t>
+  </si>
+  <si>
+    <t>x_pmb_atau_penguji_mbkm</t>
+  </si>
+  <si>
+    <t>nominal_pmb_atau_penguji_mbkm</t>
   </si>
   <si>
     <t>pmb_1_proposal_pagi</t>
@@ -217,9 +235,6 @@
     <t>nominal_pmb_company_visit</t>
   </si>
   <si>
-    <t>pembina_ukm</t>
-  </si>
-  <si>
     <t>reward_ekin</t>
   </si>
   <si>
@@ -232,9 +247,6 @@
     <t>pph_21</t>
   </si>
   <si>
-    <t>potongan_absensi</t>
-  </si>
-  <si>
     <t>potongan_bpjs</t>
   </si>
   <si>
@@ -244,10 +256,10 @@
     <t>gaji_yang_dibayar</t>
   </si>
   <si>
-    <t>diana@gmail.com</t>
-  </si>
-  <si>
-    <t>Diana</t>
+    <t>nitya@gmail.com</t>
+  </si>
+  <si>
+    <t>Nitya dewi</t>
   </si>
   <si>
     <t>Dekan</t>
@@ -261,9 +273,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
@@ -283,6 +295,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -291,6 +311,83 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -300,58 +397,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -359,25 +417,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -389,35 +430,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -434,19 +446,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,157 +620,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -646,15 +658,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -670,17 +673,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -696,6 +693,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -724,142 +736,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1198,14 +1210,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BX2"/>
+  <dimension ref="A1:CB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="1"/>
   <cols>
+    <col min="1" max="1" width="24.3" customWidth="true"/>
     <col min="5" max="5" width="15.2" customWidth="true"/>
     <col min="6" max="6" width="15.6" customWidth="true"/>
     <col min="8" max="8" width="17.4" customWidth="true"/>
@@ -1217,65 +1230,61 @@
     <col min="14" max="14" width="22.7" customWidth="true"/>
     <col min="15" max="15" width="23.8" customWidth="true"/>
     <col min="16" max="16" width="29.4" customWidth="true"/>
-    <col min="17" max="17" width="18.1" customWidth="true"/>
-    <col min="18" max="18" width="20.2" customWidth="true"/>
-    <col min="19" max="19" width="24.5" customWidth="true"/>
-    <col min="20" max="20" width="17.7" customWidth="true"/>
-    <col min="21" max="21" width="19.5" customWidth="true"/>
-    <col min="22" max="22" width="25.3" customWidth="true"/>
-    <col min="23" max="23" width="19.6" customWidth="true"/>
-    <col min="24" max="24" width="20.6" customWidth="true"/>
-    <col min="25" max="25" width="27.2" customWidth="true"/>
-    <col min="26" max="26" width="16.9" customWidth="true"/>
-    <col min="27" max="27" width="18.6" customWidth="true"/>
-    <col min="28" max="28" width="24.3" customWidth="true"/>
-    <col min="29" max="29" width="18.8" customWidth="true"/>
-    <col min="30" max="30" width="19.8" customWidth="true"/>
-    <col min="31" max="31" width="24.2" customWidth="true"/>
-    <col min="32" max="32" width="17.4" customWidth="true"/>
-    <col min="33" max="33" width="19.1" customWidth="true"/>
-    <col min="34" max="34" width="25.1" customWidth="true"/>
-    <col min="35" max="35" width="19.1" customWidth="true"/>
-    <col min="36" max="36" width="21.3" customWidth="true"/>
-    <col min="37" max="37" width="26.8" customWidth="true"/>
-    <col min="38" max="38" width="17.5" customWidth="true"/>
-    <col min="39" max="39" width="18.2" customWidth="true"/>
-    <col min="40" max="40" width="22.7" customWidth="true"/>
-    <col min="41" max="41" width="19.2" customWidth="true"/>
-    <col min="42" max="42" width="19.6" customWidth="true"/>
-    <col min="43" max="43" width="24.6" customWidth="true"/>
-    <col min="44" max="44" width="19.5" customWidth="true"/>
-    <col min="45" max="45" width="21.6" customWidth="true"/>
-    <col min="46" max="46" width="27.6" customWidth="true"/>
-    <col min="47" max="47" width="19.4" customWidth="true"/>
-    <col min="48" max="48" width="19.9" customWidth="true"/>
-    <col min="49" max="49" width="25.8" customWidth="true"/>
-    <col min="50" max="50" width="11.4" customWidth="true"/>
-    <col min="51" max="51" width="12.1" customWidth="true"/>
-    <col min="52" max="52" width="17.2" customWidth="true"/>
-    <col min="53" max="53" width="14.1" customWidth="true"/>
-    <col min="54" max="54" width="16.3" customWidth="true"/>
-    <col min="55" max="55" width="20.3" customWidth="true"/>
-    <col min="56" max="56" width="10.4" customWidth="true"/>
-    <col min="57" max="57" width="11.7" customWidth="true"/>
-    <col min="58" max="58" width="18.4" customWidth="true"/>
-    <col min="59" max="59" width="12.9" customWidth="true"/>
-    <col min="60" max="60" width="15.1" customWidth="true"/>
-    <col min="61" max="61" width="19.7" customWidth="true"/>
-    <col min="64" max="64" width="14.4" customWidth="true"/>
-    <col min="65" max="65" width="17.5" customWidth="true"/>
-    <col min="66" max="66" width="17.9" customWidth="true"/>
-    <col min="67" max="67" width="23" customWidth="true"/>
-    <col min="68" max="68" width="11.6" customWidth="true"/>
-    <col min="69" max="69" width="10.2" customWidth="true"/>
-    <col min="70" max="70" width="24.1" customWidth="true"/>
-    <col min="71" max="71" width="17.2" customWidth="true"/>
-    <col min="73" max="73" width="15.2" customWidth="true"/>
-    <col min="74" max="74" width="12.2" customWidth="true"/>
-    <col min="76" max="76" width="15.2" customWidth="true"/>
+    <col min="17" max="25" width="30.4" customWidth="true"/>
+    <col min="26" max="26" width="17.7" customWidth="true"/>
+    <col min="27" max="27" width="19.5" customWidth="true"/>
+    <col min="28" max="28" width="25.3" customWidth="true"/>
+    <col min="29" max="29" width="19.6" customWidth="true"/>
+    <col min="30" max="30" width="20.6" customWidth="true"/>
+    <col min="31" max="31" width="27.2" customWidth="true"/>
+    <col min="32" max="32" width="16.9" customWidth="true"/>
+    <col min="33" max="33" width="18.6" customWidth="true"/>
+    <col min="34" max="34" width="24.3" customWidth="true"/>
+    <col min="35" max="35" width="18.8" customWidth="true"/>
+    <col min="36" max="36" width="19.8" customWidth="true"/>
+    <col min="37" max="37" width="24.2" customWidth="true"/>
+    <col min="38" max="38" width="17.4" customWidth="true"/>
+    <col min="39" max="39" width="19.1" customWidth="true"/>
+    <col min="40" max="40" width="25.1" customWidth="true"/>
+    <col min="41" max="41" width="19.1" customWidth="true"/>
+    <col min="42" max="42" width="21.3" customWidth="true"/>
+    <col min="43" max="43" width="26.8" customWidth="true"/>
+    <col min="44" max="44" width="17.5" customWidth="true"/>
+    <col min="45" max="45" width="18.2" customWidth="true"/>
+    <col min="46" max="46" width="22.7" customWidth="true"/>
+    <col min="47" max="47" width="19.2" customWidth="true"/>
+    <col min="48" max="48" width="19.6" customWidth="true"/>
+    <col min="49" max="49" width="24.6" customWidth="true"/>
+    <col min="50" max="50" width="19.5" customWidth="true"/>
+    <col min="51" max="51" width="21.6" customWidth="true"/>
+    <col min="52" max="52" width="27.6" customWidth="true"/>
+    <col min="53" max="53" width="19.4" customWidth="true"/>
+    <col min="54" max="54" width="19.9" customWidth="true"/>
+    <col min="55" max="55" width="25.8" customWidth="true"/>
+    <col min="56" max="56" width="11.4" customWidth="true"/>
+    <col min="57" max="57" width="12.1" customWidth="true"/>
+    <col min="58" max="58" width="17.2" customWidth="true"/>
+    <col min="59" max="59" width="14.1" customWidth="true"/>
+    <col min="60" max="60" width="16.3" customWidth="true"/>
+    <col min="61" max="61" width="20.3" customWidth="true"/>
+    <col min="62" max="62" width="10.4" customWidth="true"/>
+    <col min="63" max="63" width="11.7" customWidth="true"/>
+    <col min="64" max="64" width="18.4" customWidth="true"/>
+    <col min="65" max="65" width="12.9" customWidth="true"/>
+    <col min="66" max="66" width="15.1" customWidth="true"/>
+    <col min="67" max="67" width="19.7" customWidth="true"/>
+    <col min="70" max="70" width="14.4" customWidth="true"/>
+    <col min="71" max="71" width="17.5" customWidth="true"/>
+    <col min="72" max="72" width="17.9" customWidth="true"/>
+    <col min="73" max="73" width="23" customWidth="true"/>
+    <col min="74" max="74" width="10.2" customWidth="true"/>
+    <col min="75" max="75" width="24.1" customWidth="true"/>
+    <col min="76" max="76" width="17.2" customWidth="true"/>
+    <col min="78" max="78" width="12.2" customWidth="true"/>
+    <col min="80" max="80" width="15.2" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76">
+    <row r="1" spans="1:80">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1504,25 +1513,37 @@
       <c r="BX1" t="s">
         <v>75</v>
       </c>
+      <c r="BY1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="2" spans="1:76">
+    <row r="2" spans="1:80">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="G2">
         <v>5000000</v>
@@ -1555,189 +1576,201 @@
         <v>2001</v>
       </c>
       <c r="Q2">
+        <v>26000</v>
+      </c>
+      <c r="R2">
+        <v>26</v>
+      </c>
+      <c r="S2">
+        <v>26000000</v>
+      </c>
+      <c r="T2">
+        <v>27000</v>
+      </c>
+      <c r="U2">
+        <v>27</v>
+      </c>
+      <c r="V2">
+        <v>27000000</v>
+      </c>
+      <c r="W2">
         <v>300</v>
       </c>
-      <c r="R2">
+      <c r="X2">
         <v>3</v>
       </c>
-      <c r="S2">
+      <c r="Y2">
         <v>3001</v>
       </c>
-      <c r="T2">
+      <c r="Z2">
         <v>400</v>
       </c>
-      <c r="U2">
+      <c r="AA2">
         <v>4</v>
       </c>
-      <c r="V2">
+      <c r="AB2">
         <v>4001</v>
       </c>
-      <c r="W2">
+      <c r="AC2">
         <v>500</v>
       </c>
-      <c r="X2">
+      <c r="AD2">
         <v>5</v>
       </c>
-      <c r="Y2">
+      <c r="AE2">
         <v>5001</v>
       </c>
-      <c r="Z2">
+      <c r="AF2">
         <v>600</v>
       </c>
-      <c r="AA2">
+      <c r="AG2">
         <v>6</v>
       </c>
-      <c r="AB2">
+      <c r="AH2">
         <v>6001</v>
       </c>
-      <c r="AC2">
+      <c r="AI2">
         <v>700</v>
       </c>
-      <c r="AD2">
+      <c r="AJ2">
         <v>7</v>
       </c>
-      <c r="AE2">
+      <c r="AK2">
         <v>7001</v>
       </c>
-      <c r="AF2">
+      <c r="AL2">
         <v>800</v>
       </c>
-      <c r="AG2">
+      <c r="AM2">
         <v>8</v>
       </c>
-      <c r="AH2">
+      <c r="AN2">
         <v>8001</v>
       </c>
-      <c r="AI2">
+      <c r="AO2">
         <v>900</v>
       </c>
-      <c r="AJ2">
+      <c r="AP2">
         <v>9</v>
       </c>
-      <c r="AK2">
+      <c r="AQ2">
         <v>9001</v>
       </c>
-      <c r="AL2">
+      <c r="AR2">
         <v>1010</v>
       </c>
-      <c r="AM2">
+      <c r="AS2">
         <v>10</v>
       </c>
-      <c r="AN2">
+      <c r="AT2">
         <v>10101</v>
       </c>
-      <c r="AO2">
+      <c r="AU2">
         <v>1111</v>
       </c>
-      <c r="AP2">
+      <c r="AV2">
         <v>11</v>
       </c>
-      <c r="AQ2">
+      <c r="AW2">
         <v>11111</v>
       </c>
-      <c r="AR2">
+      <c r="AX2">
         <v>1212</v>
       </c>
-      <c r="AS2">
+      <c r="AY2">
         <v>12</v>
       </c>
-      <c r="AT2">
+      <c r="AZ2">
         <v>12121</v>
       </c>
-      <c r="AU2">
+      <c r="BA2">
         <v>1313</v>
       </c>
-      <c r="AV2">
+      <c r="BB2">
         <v>13</v>
       </c>
-      <c r="AW2">
+      <c r="BC2">
         <v>13131</v>
       </c>
-      <c r="AX2">
+      <c r="BD2">
         <v>1414</v>
       </c>
-      <c r="AY2">
+      <c r="BE2">
         <v>14</v>
       </c>
-      <c r="AZ2">
+      <c r="BF2">
         <v>14141</v>
       </c>
-      <c r="BA2">
+      <c r="BG2">
         <v>1515</v>
       </c>
-      <c r="BB2">
+      <c r="BH2">
         <v>15</v>
       </c>
-      <c r="BC2">
+      <c r="BI2">
         <v>15151</v>
       </c>
-      <c r="BD2">
+      <c r="BJ2">
         <v>1616</v>
       </c>
-      <c r="BE2">
+      <c r="BK2">
         <v>16</v>
       </c>
-      <c r="BF2">
+      <c r="BL2">
         <v>16161</v>
       </c>
-      <c r="BG2">
+      <c r="BM2">
         <v>1717</v>
       </c>
-      <c r="BH2">
+      <c r="BN2">
         <v>17</v>
       </c>
-      <c r="BI2">
+      <c r="BO2">
         <v>17171</v>
       </c>
-      <c r="BJ2">
+      <c r="BP2">
         <v>1818</v>
       </c>
-      <c r="BK2">
+      <c r="BQ2">
         <v>18</v>
       </c>
-      <c r="BL2">
+      <c r="BR2">
         <v>18181</v>
       </c>
-      <c r="BM2">
+      <c r="BS2">
         <v>1919</v>
       </c>
-      <c r="BN2">
+      <c r="BT2">
         <v>19</v>
       </c>
-      <c r="BO2">
+      <c r="BU2">
         <v>19191</v>
       </c>
-      <c r="BP2">
-        <v>1500000</v>
-      </c>
-      <c r="BQ2">
+      <c r="BV2">
         <v>1600000</v>
       </c>
-      <c r="BR2">
+      <c r="BW2">
         <v>1700000</v>
       </c>
-      <c r="BS2">
+      <c r="BX2">
         <v>1800000</v>
       </c>
-      <c r="BT2">
+      <c r="BY2">
         <v>1900000</v>
       </c>
-      <c r="BU2">
-        <v>2100000</v>
-      </c>
-      <c r="BV2">
+      <c r="BZ2">
         <v>2200000</v>
       </c>
-      <c r="BW2">
+      <c r="CA2">
         <v>2300000</v>
       </c>
-      <c r="BX2">
+      <c r="CB2">
         <v>2400000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="diana@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="nitya@gmail.com" tooltip="mailto:nitya@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
menambahkan field punishment ekin untuk dosen tetap di admin
</commit_message>
<xml_diff>
--- a/public/contoh-excel/dosentetap.xlsx
+++ b/public/contoh-excel/dosentetap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>email</t>
   </si>
@@ -244,6 +244,9 @@
     <t>potongan_kas_bon</t>
   </si>
   <si>
+    <t>punishment_ekin</t>
+  </si>
+  <si>
     <t>pph_21</t>
   </si>
   <si>
@@ -256,10 +259,10 @@
     <t>gaji_yang_dibayar</t>
   </si>
   <si>
-    <t>nitya@gmail.com</t>
-  </si>
-  <si>
-    <t>Nitya dewi</t>
+    <t>buda@primakara.ac.id</t>
+  </si>
+  <si>
+    <t>Buda</t>
   </si>
   <si>
     <t>Dekan</t>
@@ -273,10 +276,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -295,6 +298,83 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -303,45 +383,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -357,13 +405,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -372,27 +413,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -402,34 +433,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -440,187 +443,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -649,15 +652,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -677,7 +671,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -731,147 +725,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1210,10 +1213,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:CB2"/>
+  <dimension ref="A1:CC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" topLeftCell="BR1" workbookViewId="0">
+      <selection activeCell="BY7" sqref="BY7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="1"/>
@@ -1279,12 +1282,12 @@
     <col min="73" max="73" width="23" customWidth="true"/>
     <col min="74" max="74" width="10.2" customWidth="true"/>
     <col min="75" max="75" width="24.1" customWidth="true"/>
-    <col min="76" max="76" width="17.2" customWidth="true"/>
-    <col min="78" max="78" width="12.2" customWidth="true"/>
-    <col min="80" max="80" width="15.2" customWidth="true"/>
+    <col min="76" max="77" width="17.2" customWidth="true"/>
+    <col min="79" max="79" width="12.2" customWidth="true"/>
+    <col min="81" max="81" width="15.2" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80">
+    <row r="1" spans="1:81">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1525,10 +1528,13 @@
       <c r="CB1" t="s">
         <v>79</v>
       </c>
+      <c r="CC1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="2" spans="1:80">
+    <row r="2" spans="1:81">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -1537,13 +1543,13 @@
         <v>2024</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G2">
         <v>5000000</v>
@@ -1756,21 +1762,24 @@
         <v>1800000</v>
       </c>
       <c r="BY2">
+        <v>266000</v>
+      </c>
+      <c r="BZ2">
         <v>1900000</v>
       </c>
-      <c r="BZ2">
+      <c r="CA2">
         <v>2200000</v>
       </c>
-      <c r="CA2">
+      <c r="CB2">
         <v>2300000</v>
       </c>
-      <c r="CB2">
+      <c r="CC2">
         <v>2400000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="nitya@gmail.com" tooltip="mailto:nitya@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="buda@primakara.ac.id" tooltip="mailto:buda@primakara.ac.id"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>